<commit_message>
refactor: added blank lines between classes in properties sheet
</commit_message>
<xml_diff>
--- a/tests/tests_unit/rules/test_exporters/test.xlsx
+++ b/tests/tests_unit/rules/test_exporters/test.xlsx
@@ -582,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -891,47 +891,22 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WindTurbine</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>power:WindTurbine</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>power:WindTurbine(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -941,16 +916,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ratedPower</t>
+          <t>manufacturer</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -962,7 +937,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>ratedPower</t>
+          <t>manufacturer</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -972,7 +947,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>ratedPower</t>
+          <t>manufacturer</t>
         </is>
       </c>
     </row>
@@ -984,7 +959,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hubHeight</t>
+          <t>ratedPower</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1005,7 +980,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>hubHeight</t>
+          <t>ratedPower</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1015,7 +990,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>hubHeight</t>
+          <t>ratedPower</t>
         </is>
       </c>
     </row>
@@ -1027,21 +1002,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>arrayCableConnection</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>hubHeight</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>power:ArrayCable(version=0.1.0)</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1053,7 +1023,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>arrayCableConnection</t>
+          <t>hubHeight</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1063,7 +1033,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>arrayCableConnection</t>
+          <t>hubHeight</t>
         </is>
       </c>
     </row>
@@ -1075,12 +1045,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>lifeExpectancy</t>
+          <t>arrayCableConnection</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>int32</t>
+          <t>power:ArrayCable(version=0.1.0)</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -1096,7 +1071,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>lifeExpectancy</t>
+          <t>arrayCableConnection</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1106,29 +1081,24 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>lifeExpectancy</t>
+          <t>arrayCableConnection</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PowerLine</t>
+          <t>WindTurbine</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>voltageLevel</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>lifeExpectancy</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>power:VoltageLevel(version=0.1.0)</t>
+          <t>int32</t>
         </is>
       </c>
       <c r="G12" t="b">
@@ -1139,72 +1109,42 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>power:PowerLine</t>
+          <t>power:WindTurbine</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>voltageLevel</t>
+          <t>lifeExpectancy</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>power:PowerLine(version=0.1.0)</t>
+          <t>power:WindTurbine(version=0.1.0)</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>voltageLevel</t>
+          <t>lifeExpectancy</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>PowerLine</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>power:MultiLineString(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>power:PowerLine</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>power:PowerLine(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1214,16 +1154,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>currentVoltage</t>
+          <t>voltageLevel</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>timeseries</t>
+          <t>power:VoltageLevel(version=0.1.0)</t>
         </is>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -1235,7 +1180,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>currentVoltage</t>
+          <t>voltageLevel</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1245,127 +1190,118 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>currentVoltage</t>
+          <t>voltageLevel</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Substation</t>
+          <t>PowerLine</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>geoLocation</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>power:MultiLineString(version=0.1.0)</t>
         </is>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>power:Substation</t>
+          <t>power:PowerLine</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>geoLocation</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>power:Substation(version=0.1.0)</t>
+          <t>power:PowerLine(version=0.1.0)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>geoLocation</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Substation</t>
+          <t>PowerLine</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>currentVoltage</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>power:Substation</t>
+          <t>power:PowerLine</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>currentVoltage</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>power:Substation(version=0.1.0)</t>
+          <t>power:PowerLine(version=0.1.0)</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>currentVoltage</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Substation</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>disconnectSwitch</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>multiedge</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>power:DisconnectSwitch(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>power:Substation(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>disconnectSwitch</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1375,17 +1311,28 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>circuitBreaker</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>multiedge</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>power:CircuitBreaker(version=0.1.0)</t>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>power:Substation</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1395,7 +1342,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>circuitBreaker</t>
+          <t>name</t>
         </is>
       </c>
     </row>
@@ -1407,17 +1354,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>currentTransformer</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>multiedge</t>
+          <t>location</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>power:CurrentTransformer(version=0.1.0)</t>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>power:Substation</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>location</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1427,7 +1385,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>currentTransformer</t>
+          <t>location</t>
         </is>
       </c>
     </row>
@@ -1439,33 +1397,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>mainTransformer</t>
+          <t>disconnectSwitch</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>power:VoltageTransformer(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>power:Substation</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>mainTransformer</t>
+          <t>power:DisconnectSwitch(version=0.1.0)</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1475,7 +1417,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>mainTransformer</t>
+          <t>disconnectSwitch</t>
         </is>
       </c>
     </row>
@@ -1487,33 +1429,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>primaryPowerLine</t>
+          <t>circuitBreaker</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>power:PowerLine(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>power:Substation</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>primaryPowerLine</t>
+          <t>power:CircuitBreaker(version=0.1.0)</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1523,7 +1449,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>primaryPowerLine</t>
+          <t>circuitBreaker</t>
         </is>
       </c>
     </row>
@@ -1535,33 +1461,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>secondaryPowerLine</t>
+          <t>currentTransformer</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>power:PowerLine(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>power:Substation</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>secondaryPowerLine</t>
+          <t>power:CurrentTransformer(version=0.1.0)</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1571,7 +1481,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>secondaryPowerLine</t>
+          <t>currentTransformer</t>
         </is>
       </c>
     </row>
@@ -1583,16 +1493,21 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>primaryVoltage</t>
+          <t>mainTransformer</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>timeseries</t>
+          <t>power:VoltageTransformer(version=0.1.0)</t>
         </is>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1604,7 +1519,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>primaryVoltage</t>
+          <t>mainTransformer</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -1614,7 +1529,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>primaryVoltage</t>
+          <t>mainTransformer</t>
         </is>
       </c>
     </row>
@@ -1626,16 +1541,21 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>secondaryVoltage</t>
+          <t>primaryPowerLine</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>timeseries</t>
+          <t>power:PowerLine(version=0.1.0)</t>
         </is>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -1647,7 +1567,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>secondaryVoltage</t>
+          <t>primaryPowerLine</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -1657,104 +1577,115 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>secondaryVoltage</t>
+          <t>primaryPowerLine</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>OffshoreSubstation</t>
+          <t>Substation</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>primaryPowerLine</t>
+          <t>secondaryPowerLine</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>multiedge</t>
+          <t>direct</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>power:ArrayCable(version=0.1.0)</t>
+          <t>power:PowerLine(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>power:Substation</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>secondaryPowerLine</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>power:OffshoreSubstation(version=0.1.0)</t>
+          <t>power:Substation(version=0.1.0)</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>primaryPowerLine</t>
+          <t>secondaryPowerLine</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>OffshoreSubstation</t>
+          <t>Substation</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>secondaryPowerLine</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>primaryVoltage</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>power:ExportCable(version=0.1.0)</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>power:OffshoreSubstation</t>
+          <t>power:Substation</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>secondaryPowerLine</t>
+          <t>primaryVoltage</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>power:OffshoreSubstation(version=0.1.0)</t>
+          <t>power:Substation(version=0.1.0)</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>secondaryPowerLine</t>
+          <t>primaryVoltage</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>EnergyArea</t>
+          <t>Substation</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>secondaryVoltage</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="G27" t="b">
@@ -1765,333 +1696,289 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>power:EnergyArea</t>
+          <t>power:Substation</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>secondaryVoltage</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>power:EnergyArea(version=0.1.0)</t>
+          <t>power:Substation(version=0.1.0)</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>secondaryVoltage</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>EnergyArea</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>power:Polygon(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>power:EnergyArea</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>power:EnergyArea(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>geoLocation</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EnergyArea</t>
+          <t>OffshoreSubstation</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ratedPower</t>
+          <t>primaryPowerLine</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>power:EnergyArea</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>ratedPower</t>
+          <t>power:ArrayCable(version=0.1.0)</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>power:EnergyArea(version=0.1.0)</t>
+          <t>power:OffshoreSubstation(version=0.1.0)</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>ratedPower</t>
+          <t>primaryPowerLine</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EnergyArea</t>
+          <t>OffshoreSubstation</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>activePower</t>
+          <t>secondaryPowerLine</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>timeseries</t>
+          <t>power:ExportCable(version=0.1.0)</t>
         </is>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>power:EnergyArea</t>
+          <t>power:OffshoreSubstation</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>activePower</t>
+          <t>secondaryPowerLine</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>power:EnergyArea(version=0.1.0)</t>
+          <t>power:OffshoreSubstation(version=0.1.0)</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>activePower</t>
+          <t>secondaryPowerLine</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>WindFarm</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>windTurbines</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>multiedge</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>power:WindTurbine(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>power:WindFarm(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>windTurbines</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>WindFarm</t>
+          <t>EnergyArea</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>substation</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>power:OffshoreSubstation(version=0.1.0)</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>power:WindFarm</t>
+          <t>power:EnergyArea</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>name</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>power:WindFarm(version=0.1.0)</t>
+          <t>power:EnergyArea(version=0.1.0)</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>name</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>WindFarm</t>
+          <t>EnergyArea</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>arrayCable</t>
+          <t>geoLocation</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>multiedge</t>
+          <t>direct</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>power:ArrayCable(version=0.1.0)</t>
+          <t>power:Polygon(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>power:EnergyArea</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>geoLocation</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>power:WindFarm(version=0.1.0)</t>
+          <t>power:EnergyArea(version=0.1.0)</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>arrayCable</t>
+          <t>geoLocation</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>WindFarm</t>
+          <t>EnergyArea</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>exportCable</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>ratedPower</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>power:ExportCable(version=0.1.0)</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>power:WindFarm</t>
+          <t>power:EnergyArea</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>exportCable</t>
+          <t>ratedPower</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>power:WindFarm(version=0.1.0)</t>
+          <t>power:EnergyArea(version=0.1.0)</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>exportCable</t>
+          <t>ratedPower</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Factory</t>
+          <t>EnergyArea</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>activePower</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="G35" t="b">
@@ -2102,318 +1989,273 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>power:Factory</t>
+          <t>power:EnergyArea</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>activePower</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>power:Factory(version=0.1.0)</t>
+          <t>power:EnergyArea(version=0.1.0)</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>activePower</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Factory</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>power:Point(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>power:Factory</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>power:Factory(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Factory</t>
+          <t>WindFarm</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>load</t>
+          <t>windTurbines</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>timeseries</t>
-        </is>
-      </c>
-      <c r="G37" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>power:Factory</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>load</t>
+          <t>power:WindTurbine(version=0.1.0)</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>power:Factory(version=0.1.0)</t>
+          <t>power:WindFarm(version=0.1.0)</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>load</t>
+          <t>windTurbines</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>WindFarm</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>latitude</t>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>direct</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>power:OffshoreSubstation(version=0.1.0)</t>
         </is>
       </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>power:Point</t>
+          <t>power:WindFarm</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>latitude</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>power:Point(version=0.1.0)</t>
+          <t>power:WindFarm(version=0.1.0)</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>latitude</t>
+          <t>substation</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>WindFarm</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>longitude</t>
+          <t>arrayCable</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>multiedge</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>power:Point</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>longitude</t>
+          <t>power:ArrayCable(version=0.1.0)</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>power:Point(version=0.1.0)</t>
+          <t>power:WindFarm(version=0.1.0)</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>longitude</t>
+          <t>arrayCable</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MultiLineString</t>
+          <t>WindFarm</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>point</t>
+          <t>exportCable</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>multiedge</t>
+          <t>direct</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>power:Point(version=0.1.0)</t>
+          <t>power:ExportCable(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>power:WindFarm</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>exportCable</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>power:MultiLineString(version=0.1.0)</t>
+          <t>power:WindFarm(version=0.1.0)</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>point</t>
+          <t>exportCable</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Polygon</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>point</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>multiedge</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>power:Point(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>power:Polygon(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>point</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CurrentTransformer</t>
+          <t>Factory</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>power:CurrentTransformer</t>
+          <t>power:Factory</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>name</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>power:CurrentTransformer(version=0.1.0)</t>
+          <t>power:Factory(version=0.1.0)</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>name</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>VoltageTransformer</t>
+          <t>Factory</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>outputVoltageLevel</t>
+          <t>location</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2423,7 +2265,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>power:VoltageLevel(version=0.1.0)</t>
+          <t>power:Point(version=0.1.0)</t>
         </is>
       </c>
       <c r="G43" t="b">
@@ -2434,125 +2276,95 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>power:VoltageTransformer</t>
+          <t>power:Factory</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>outputVoltageLevel</t>
+          <t>location</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>power:VoltageTransformer(version=0.1.0)</t>
+          <t>power:Factory(version=0.1.0)</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>outputVoltageLevel</t>
+          <t>location</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>VoltageTransformer</t>
+          <t>Factory</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>inputVoltageLevel</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>direct</t>
+          <t>load</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>power:VoltageLevel(version=0.1.0)</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>power:VoltageTransformer</t>
+          <t>power:Factory</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>inputVoltageLevel</t>
+          <t>load</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>power:VoltageTransformer(version=0.1.0)</t>
+          <t>power:Factory(version=0.1.0)</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>inputVoltageLevel</t>
+          <t>load</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>VoltageLevel</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>maxLevel</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="G45" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>power:VoltageLevel</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>maxLevel</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>power:VoltageLevel(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>maxLevel</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ExportCable</t>
+          <t>Point</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>length</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2561,41 +2373,41 @@
         </is>
       </c>
       <c r="G46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>power:ExportCable</t>
+          <t>power:Point</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>length</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>power:ExportCable(version=0.1.0)</t>
+          <t>power:Point(version=0.1.0)</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>length</t>
+          <t>latitude</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CircuitBreaker</t>
+          <t>Point</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>longitude</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2604,113 +2416,607 @@
         </is>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>power:CircuitBreaker</t>
+          <t>power:Point</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>longitude</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>power:CircuitBreaker(version=0.1.0)</t>
+          <t>power:Point(version=0.1.0)</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>maxCapacity</t>
+          <t>longitude</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ArrayCable</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="G48" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>power:ArrayCable</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>power:ArrayCable(version=0.1.0)</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>MultiLineString</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>point</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>multiedge</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>power:Point(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>power:MultiLineString(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>point</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Polygon</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>point</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>multiedge</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>power:Point(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>power:Polygon(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>point</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CurrentTransformer</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>power:CurrentTransformer</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>power:CurrentTransformer(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>VoltageTransformer</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>outputVoltageLevel</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>power:VoltageLevel(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>power:VoltageTransformer</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>outputVoltageLevel</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>power:VoltageTransformer(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>outputVoltageLevel</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>VoltageTransformer</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>inputVoltageLevel</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>power:VoltageLevel(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>power:VoltageTransformer</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>inputVoltageLevel</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>power:VoltageTransformer(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>inputVoltageLevel</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>VoltageLevel</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>maxLevel</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>power:VoltageLevel</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>maxLevel</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>power:VoltageLevel(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>maxLevel</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ExportCable</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>power:ExportCable</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>power:ExportCable(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>CircuitBreaker</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>power:CircuitBreaker</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>power:CircuitBreaker(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>maxCapacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ArrayCable</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>power:ArrayCable</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>power:ArrayCable(version=0.1.0)</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>DisconnectSwitch</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>maxCapacity</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>float64</t>
         </is>
       </c>
-      <c r="G49" t="b">
+      <c r="G66" t="b">
         <v>1</v>
       </c>
-      <c r="H49" t="b">
-        <v>0</v>
-      </c>
-      <c r="K49" t="inlineStr">
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>power:DisconnectSwitch</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
+      <c r="L66" t="inlineStr">
         <is>
           <t>maxCapacity</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="M66" t="inlineStr">
         <is>
           <t>power:DisconnectSwitch(version=0.1.0)</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr">
+      <c r="N66" t="inlineStr">
         <is>
           <t>maxCapacity</t>
         </is>

</xml_diff>